<commit_message>
Fixed the run mode issues.
</commit_message>
<xml_diff>
--- a/src/test/resources/com/w2a/excel/testdata.xlsx
+++ b/src/test/resources/com/w2a/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\posta\eclipse-workspace\PageObjectModelZoho\src\test\resources\com\w2a\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70AC99F-ED14-40D6-8088-C7B75D2DC3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA12B03-E1FA-4E14-81E6-A7670B39E1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{F36CACDF-48E3-4E29-8EB3-C9ACD8ED91B8}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{F36CACDF-48E3-4E29-8EB3-C9ACD8ED91B8}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>TCID</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>ZohoLoginTest</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>highlandasia@gmail.com</t>
@@ -441,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C4E091-E60D-4AF3-97C2-6DC4584481B7}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,15 +456,15 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -495,12 +492,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93786EF7-B594-4891-B411-CF57D15E3531}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -526,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +536,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -547,7 +544,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -555,10 +552,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>